<commit_message>
Experiments progress…t-SNE almost done.
</commit_message>
<xml_diff>
--- a/PaperNeural/Results/ResultsMar2017-t-SNE_MI_2000_LR_700_PE_39.xlsx
+++ b/PaperNeural/Results/ResultsMar2017-t-SNE_MI_2000_LR_700_PE_39.xlsx
@@ -7638,34 +7638,56 @@
       <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>26.31578947368421</v>
+      </c>
       <c r="I24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.9777777777777777</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>4.093567251461988</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.125</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -7674,9 +7696,15 @@
       <c r="I25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.9722222222222222</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.027777777777777776</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -7688,9 +7716,15 @@
       <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -7699,9 +7733,15 @@
       <c r="I26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.018518518518518517</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.9259259259259259</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -8215,34 +8255,56 @@
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>36.84210526315789</v>
+      </c>
       <c r="I18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.044444444444444446</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>14.619883040935672</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.125</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -8251,9 +8313,15 @@
       <c r="I19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.05555555555555555</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -8265,9 +8333,15 @@
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -8276,9 +8350,15 @@
       <c r="I20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.037037037037037035</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>0.8518518518518519</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -8349,34 +8429,56 @@
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.2</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>31.57894736842105</v>
+      </c>
       <c r="I24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>10.526315789473683</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.25</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -8385,9 +8487,15 @@
       <c r="I25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.041666666666666664</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.041666666666666664</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -8399,9 +8507,15 @@
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -8410,9 +8524,15 @@
       <c r="I26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.037037037037037035</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.07407407407407407</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.8888888888888888</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -8926,34 +9046,56 @@
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>15.789473684210526</v>
+      </c>
       <c r="I18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>0.9777777777777777</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>2.923976608187134</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -8962,9 +9104,15 @@
       <c r="I19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.027777777777777776</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.013888888888888888</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -8976,9 +9124,15 @@
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -8987,9 +9141,15 @@
       <c r="I20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.018518518518518517</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>0.9814814814814815</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -9060,34 +9220,56 @@
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>21.052631578947366</v>
+      </c>
       <c r="I24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>4.093567251461988</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -9096,9 +9278,15 @@
       <c r="I25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.9722222222222222</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.027777777777777776</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -9110,9 +9298,15 @@
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -9121,9 +9315,15 @@
       <c r="I26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.9444444444444444</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -9637,34 +9837,56 @@
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>26.31578947368421</v>
+      </c>
       <c r="I18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>0.9777777777777777</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>2.3391812865497075</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.25</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -9673,9 +9895,15 @@
       <c r="I19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.027777777777777776</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>0.9722222222222222</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -9687,9 +9915,15 @@
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -9698,9 +9932,15 @@
       <c r="I20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.018518518518518517</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>0.9814814814814815</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -9771,34 +10011,56 @@
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.2</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>36.84210526315789</v>
+      </c>
       <c r="I24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>5.847953216374268</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.25</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -9807,9 +10069,15 @@
       <c r="I25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.9722222222222222</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.027777777777777776</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -9821,9 +10089,15 @@
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -9832,9 +10106,15 @@
       <c r="I26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.037037037037037035</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.07407407407407407</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.8888888888888888</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -10344,34 +10624,56 @@
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>21.052631578947366</v>
+      </c>
       <c r="I18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.044444444444444446</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>1.1695906432748537</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.125</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -10380,9 +10682,15 @@
       <c r="I19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -10394,9 +10702,15 @@
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -10405,9 +10719,15 @@
       <c r="I20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>1.0</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -10478,34 +10798,56 @@
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>21.052631578947366</v>
+      </c>
       <c r="I24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.9777777777777777</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>5.263157894736842</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -10514,9 +10856,15 @@
       <c r="I25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.041666666666666664</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -10528,9 +10876,15 @@
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -10539,9 +10893,15 @@
       <c r="I26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.018518518518518517</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.07407407407407407</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.9074074074074074</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -11055,34 +11415,56 @@
       <c r="B18" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>21.052631578947366</v>
+      </c>
       <c r="I18" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>0.5847953216374269</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.125</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -11091,9 +11473,15 @@
       <c r="I19" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -11105,9 +11493,15 @@
       <c r="B20" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -11116,9 +11510,15 @@
       <c r="I20" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.018518518518518517</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>0.9814814814814815</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -11189,34 +11589,56 @@
       <c r="B24" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>36.84210526315789</v>
+      </c>
       <c r="I24" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>0.9777777777777777</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>3.508771929824561</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.375</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -11225,9 +11647,15 @@
       <c r="I25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.013888888888888888</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.9722222222222222</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.013888888888888888</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -11239,9 +11667,15 @@
       <c r="B26" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.8333333333333334</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -11250,9 +11684,15 @@
       <c r="I26" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.037037037037037035</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.018518518518518517</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.9444444444444444</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>
@@ -11775,34 +12215,56 @@
       <c r="B18" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
+      <c r="C18" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="63" t="n">
+        <v>21.052631578947366</v>
+      </c>
       <c r="I18" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
+      <c r="J18" s="40" t="n">
+        <v>0.9777777777777777</v>
+      </c>
+      <c r="K18" s="40" t="n">
+        <v>0.022222222222222223</v>
+      </c>
+      <c r="L18" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="63"/>
+      <c r="N18" s="63" t="n">
+        <v>0.5847953216374269</v>
+      </c>
     </row>
     <row r="19" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="61"/>
       <c r="B19" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="C19" s="40" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E19" s="40" t="n">
+        <v>0.125</v>
+      </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
         <v>#DIV/0!</v>
@@ -11811,9 +12273,15 @@
       <c r="I19" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="J19" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K19" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="L19" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M19" s="3" t="e">
         <f>100*K19/(SUM(J19:L19))</f>
         <v>#DIV/0!</v>
@@ -11825,9 +12293,15 @@
       <c r="B20" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
+      <c r="C20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
         <v>#DIV/0!</v>
@@ -11836,9 +12310,15 @@
       <c r="I20" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
+      <c r="J20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K20" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L20" s="40" t="n">
+        <v>1.0</v>
+      </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
         <v>#DIV/0!</v>
@@ -11909,34 +12389,56 @@
       <c r="B24" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+      <c r="C24" s="40" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E24" s="40" t="n">
+        <v>0.2</v>
+      </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="63"/>
+      <c r="G24" s="63" t="n">
+        <v>21.052631578947366</v>
+      </c>
       <c r="I24" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L24" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N24" s="63"/>
+      <c r="N24" s="63" t="n">
+        <v>3.508771929824561</v>
+      </c>
     </row>
     <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="61"/>
       <c r="B25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" s="40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E25" s="40" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
         <v>#DIV/0!</v>
@@ -11945,9 +12447,15 @@
       <c r="I25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="J25" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K25" s="40" t="n">
+        <v>0.9722222222222222</v>
+      </c>
+      <c r="L25" s="40" t="n">
+        <v>0.027777777777777776</v>
+      </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
         <v>#DIV/0!</v>
@@ -11959,9 +12467,15 @@
       <c r="B26" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="C26" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D26" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E26" s="40" t="n">
+        <v>0.5</v>
+      </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
         <v>#DIV/0!</v>
@@ -11970,9 +12484,15 @@
       <c r="I26" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
+      <c r="J26" s="40" t="n">
+        <v>0.018518518518518517</v>
+      </c>
+      <c r="K26" s="40" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="L26" s="40" t="n">
+        <v>0.9259259259259259</v>
+      </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
         <v>#DIV/0!</v>

</xml_diff>